<commit_message>
clustering and color changes in files main.py clusterChart component and clustering.py though clustering.py change won't affect code.
</commit_message>
<xml_diff>
--- a/backend/uploads/ASSY BOM .xlsx
+++ b/backend/uploads/ASSY BOM .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vedan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INEEXTPSR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C9E3BE-71FE-4EE1-87A2-34F8921C3A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4B60CF-B850-4567-97EA-3D00B0A642DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{39774554-9A1B-42E4-82AB-B3418FDDAB44}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{39774554-9A1B-42E4-82AB-B3418FDDAB44}"/>
   </bookViews>
   <sheets>
     <sheet name="3 Assy Bom" sheetId="1" r:id="rId1"/>
@@ -68,6 +68,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -391,9 +393,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -406,6 +405,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1380,8 +1382,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C116"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1403,13 +1405,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="14">
         <v>0</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1854,13 +1856,13 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="14">
         <v>0</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="15">
         <v>1</v>
       </c>
     </row>
@@ -2261,13 +2263,13 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B80" s="10">
+      <c r="B80" s="14">
         <v>0</v>
       </c>
-      <c r="C80" s="11">
+      <c r="C80" s="15">
         <v>1</v>
       </c>
     </row>
@@ -2679,7 +2681,7 @@
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2725,8 +2727,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2763,46 +2765,46 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="9">
         <v>0.88</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="11">
         <v>30</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="F4" s="15">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="F4" s="12">
         <v>4</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">

</xml_diff>